<commit_message>
I have modified the list
</commit_message>
<xml_diff>
--- a/Shopping_List.xlsx
+++ b/Shopping_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT-Demo\CFO1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CF172F-C209-4E1A-A24C-4E47C911F61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0D1747-9E64-44DB-8139-770284096BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dairy" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Milk</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>Turkey</t>
+  </si>
+  <si>
+    <t>Strawberries</t>
+  </si>
+  <si>
+    <t>Ananas</t>
+  </si>
+  <si>
+    <t>Kiwis</t>
   </si>
 </sst>
 </file>
@@ -361,6 +370,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F950A2C2-147E-400C-9EBF-680462D9111C}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB242E0D-C90C-4B04-823C-177862BF2A2B}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -371,8 +435,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F950A2C2-147E-400C-9EBF-680462D9111C}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D383AC8-8528-41E5-85BA-F8FAB1884BA2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6D4B6F-559B-429B-A583-759C0B85209E}">
   <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -383,66 +459,17 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB242E0D-C90C-4B04-823C-177862BF2A2B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D383AC8-8528-41E5-85BA-F8FAB1884BA2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6D4B6F-559B-429B-A583-759C0B85209E}">
-  <dimension ref="B2:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>